<commit_message>
IoV Revised 929v003: 增加6个弹箱/弹盒 3105 - 9x90mm MEN, box 3106 - 9mm Metal Storm crate 3107 - 25x59mm, B crate 3108 - 20x42mm, HE crate 3109 - 12Ga MAUL Buckshot crate 3110 - 12Ga MAUL Slug crate
</commit_message>
<xml_diff>
--- a/Data-IoV_Revised/_Docs/IoV_Revised_Modify_log.xlsx
+++ b/Data-IoV_Revised/_Docs/IoV_Revised_Modify_log.xlsx
@@ -5,14 +5,15 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\00_TEMP\00_Download\Data-IoV\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Green_Game\Jagged Alliance 2\JA2+v1.13+MODs_2014\Data-IoV\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20760" windowHeight="11265"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20760" windowHeight="11265" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="弹匣相关" sheetId="1" r:id="rId1"/>
+    <sheet name="物品增加" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="175">
   <si>
     <t>原ID</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -541,6 +542,36 @@
       </rPr>
       <t>（原则是某类型某个数量保证有一个在1970内）</t>
     </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>新加物品ID</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Name(暂定3105~3500为新增弹类用)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>9x90mm MEN, box</t>
+  </si>
+  <si>
+    <t>9mm Metal Storm crate</t>
+  </si>
+  <si>
+    <t>25x59mm, B crate</t>
+  </si>
+  <si>
+    <t>20x42mm, HE crate</t>
+  </si>
+  <si>
+    <t>12Ga MAUL Buckshot crate</t>
+  </si>
+  <si>
+    <t>12Ga MAUL Slug crate</t>
+  </si>
+  <si>
+    <t>弹匣</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -598,12 +629,24 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="9">
@@ -700,7 +743,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -757,6 +800,12 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1040,7 +1089,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K91"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
@@ -2984,4 +3033,91 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="11.625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="44.25" style="2" customWidth="1"/>
+    <col min="3" max="16384" width="9" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A1" s="19" t="s">
+        <v>174</v>
+      </c>
+      <c r="B1" s="19"/>
+    </row>
+    <row r="2" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A2" s="20" t="s">
+        <v>166</v>
+      </c>
+      <c r="B2" s="20" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3" s="3">
+        <v>3105</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A4" s="3">
+        <v>3106</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A5" s="3">
+        <v>3107</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A6" s="3">
+        <v>3108</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A7" s="3">
+        <v>3109</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A8" s="3">
+        <v>3110</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>173</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:B1"/>
+  </mergeCells>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>